<commit_message>
patient_id & encounter_id fix
</commit_message>
<xml_diff>
--- a/ch/docs/source/Data validation issues.xlsx
+++ b/ch/docs/source/Data validation issues.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vihangamagarwal/Documents/DataThoughts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vihangamagarwal/code/century_health/century_health/ch/docs/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66441DF-B999-0548-BC7E-81DB6BB58B70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0C0D9C-B46C-014C-A41A-BBD4D8B453D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{F8B68C2A-ADE3-9B45-8499-791D23C1BC07}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
   <si>
     <t>Patients</t>
   </si>
@@ -119,6 +119,15 @@
   </si>
   <si>
     <t>Updated to PATIENT_ID</t>
+  </si>
+  <si>
+    <t>Patient id case is not consistent across datasets</t>
+  </si>
+  <si>
+    <t>Encounter id case is not consistent across datasets</t>
+  </si>
+  <si>
+    <t>Updated to ENCOUNTER_ID</t>
   </si>
 </sst>
 </file>
@@ -174,8 +183,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B1A1DC99-DB95-E54D-B23B-95E34AA76ECC}" name="Table1" displayName="Table1" ref="A1:E13" totalsRowShown="0">
-  <autoFilter ref="A1:E13" xr:uid="{B1A1DC99-DB95-E54D-B23B-95E34AA76ECC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B1A1DC99-DB95-E54D-B23B-95E34AA76ECC}" name="Table1" displayName="Table1" ref="A1:E15" totalsRowShown="0">
+  <autoFilter ref="A1:E15" xr:uid="{B1A1DC99-DB95-E54D-B23B-95E34AA76ECC}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{FA6E4129-302F-304E-8985-1CDB5A2648FA}" name="#">
       <calculatedColumnFormula>A1+1</calculatedColumnFormula>
@@ -486,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D3A59A-AEB5-114C-A7FF-77381729323E}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -552,7 +561,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
-        <f t="shared" ref="A4:A13" si="0">A3+1</f>
+        <f t="shared" ref="A4:A15" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -728,6 +737,42 @@
       </c>
       <c r="E13" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>